<commit_message>
added aura to legendaries
</commit_message>
<xml_diff>
--- a/Pokemon Supply Distribution.xlsx
+++ b/Pokemon Supply Distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ellaine Grace Salisi\Desktop\git\rumble\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\00 - Projects\Dev\rumble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25CFA6-7C59-4C0C-8145-5181D77FFA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0690E5-CA23-404E-8508-F2270FD539EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="2145" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{C5DC818E-8AB9-4D02-86E9-8C9248B295A5}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C5DC818E-8AB9-4D02-86E9-8C9248B295A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -282,21 +282,9 @@
     <t>celestik</t>
   </si>
   <si>
-    <t>jiratik</t>
-  </si>
-  <si>
-    <t>draco</t>
-  </si>
-  <si>
-    <t>articane</t>
-  </si>
-  <si>
     <t>dagitab</t>
   </si>
   <si>
-    <t>moltyte</t>
-  </si>
-  <si>
     <t>protwo</t>
   </si>
   <si>
@@ -415,6 +403,18 @@
   </si>
   <si>
     <t>watts</t>
+  </si>
+  <si>
+    <t>quartzan</t>
+  </si>
+  <si>
+    <t>azrure</t>
+  </si>
+  <si>
+    <t>diwa</t>
+  </si>
+  <si>
+    <t>milid</t>
   </si>
 </sst>
 </file>
@@ -881,9 +881,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>14</v>
       </c>
@@ -891,7 +891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -909,7 +909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -927,7 +927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -945,7 +945,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -963,7 +963,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6">
         <f>SUM(E2:E5)</f>
         <v>1000</v>
@@ -979,21 +979,21 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>p.hi proto</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>p.hi celestik</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
@@ -1102,14 +1102,14 @@
       </c>
       <c r="I5" t="str">
         <f>LOWER(_xlfn.CONCAT("p.create ",Table1[[#This Row],[ID]]," ",Table1[[#This Row],[Column1]]," ",Table1[[#This Row],[Rarity]]," ",1))</f>
-        <v>p.create 385 jiratik mythical 1</v>
+        <v>p.create 385 diwa mythical 1</v>
       </c>
       <c r="J5" t="str">
         <f>LOWER(_xlfn.CONCAT("p.hi ",Table1[[#This Row],[Column1]]))</f>
-        <v>p.hi jiratik</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>p.hi diwa</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>65</v>
@@ -1130,14 +1130,14 @@
       </c>
       <c r="I6" t="str">
         <f>LOWER(_xlfn.CONCAT("p.create ",Table1[[#This Row],[ID]]," ",Table1[[#This Row],[Column1]]," ",Table1[[#This Row],[Rarity]]," ",1))</f>
-        <v>p.create 491 draco mythical 1</v>
+        <v>p.create 491 milid mythical 1</v>
       </c>
       <c r="J6" t="str">
         <f>LOWER(_xlfn.CONCAT("p.hi ",Table1[[#This Row],[Column1]]))</f>
-        <v>p.hi draco</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>p.hi milid</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>66</v>
@@ -1158,14 +1158,14 @@
       </c>
       <c r="I7" t="str">
         <f>LOWER(_xlfn.CONCAT("p.create ",Table1[[#This Row],[ID]]," ",Table1[[#This Row],[Column1]]," ",Table1[[#This Row],[Rarity]]," ",1))</f>
-        <v>p.create 144 articane legendary 1</v>
+        <v>p.create 144 quartzan legendary 1</v>
       </c>
       <c r="J7" t="str">
         <f>LOWER(_xlfn.CONCAT("p.hi ",Table1[[#This Row],[Column1]]))</f>
-        <v>p.hi articane</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>p.hi quartzan</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>67</v>
@@ -1193,7 +1193,7 @@
         <v>p.hi dagitab</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>68</v>
@@ -1214,14 +1214,14 @@
       </c>
       <c r="I9" t="str">
         <f>LOWER(_xlfn.CONCAT("p.create ",Table1[[#This Row],[ID]]," ",Table1[[#This Row],[Column1]]," ",Table1[[#This Row],[Rarity]]," ",1))</f>
-        <v>p.create 146 moltyte legendary 1</v>
+        <v>p.create 146 azrure legendary 1</v>
       </c>
       <c r="J9" t="str">
         <f>LOWER(_xlfn.CONCAT("p.hi ",Table1[[#This Row],[Column1]]))</f>
-        <v>p.hi moltyte</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>p.hi azrure</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>62</v>
@@ -1249,7 +1249,7 @@
         <v>p.hi protwo</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>69</v>
@@ -1277,7 +1277,7 @@
         <v>p.hi rhinome</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>58</v>
@@ -1305,7 +1305,7 @@
         <v>p.hi jaguatone</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>59</v>
@@ -1333,7 +1333,7 @@
         <v>p.hi vopari</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>48</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>60</v>
@@ -1361,7 +1361,7 @@
         <v>p.hi saha</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>70</v>
@@ -1389,7 +1389,7 @@
         <v>p.hi luwi</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>55</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>58</v>
@@ -1417,7 +1417,7 @@
         <v>p.hi voltran</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>59</v>
@@ -1445,7 +1445,7 @@
         <v>p.hi hypony</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>71</v>
@@ -1473,7 +1473,7 @@
         <v>p.hi venok</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>58</v>
@@ -1501,7 +1501,7 @@
         <v>p.hi alphatross</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>60</v>
@@ -1529,15 +1529,15 @@
         <v>p.hi specinea</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>58</v>
@@ -1557,7 +1557,7 @@
         <v>p.hi mavi</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>61</v>
@@ -1585,7 +1585,7 @@
         <v>p.hi salamazel</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>59</v>
@@ -1613,7 +1613,7 @@
         <v>p.hi blazter</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>60</v>
@@ -1641,7 +1641,7 @@
         <v>p.hi sid</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>27</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>60</v>
@@ -1669,7 +1669,7 @@
         <v>p.hi tuko</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>60</v>
@@ -1697,7 +1697,7 @@
         <v>p.hi allily</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>35</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>60</v>
@@ -1725,7 +1725,7 @@
         <v>p.hi keru-keru</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>30</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>59</v>
@@ -1753,7 +1753,7 @@
         <v>p.hi pen-pen</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>31</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>59</v>
@@ -1781,7 +1781,7 @@
         <v>p.hi polydent</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>58</v>
@@ -1809,7 +1809,7 @@
         <v>p.hi watts</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>36</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>61</v>
@@ -1837,7 +1837,7 @@
         <v>p.hi quiltile</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>45</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>58</v>
@@ -1865,7 +1865,7 @@
         <v>p.hi luxious</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>61</v>
@@ -1893,7 +1893,7 @@
         <v>p.hi menggay</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>58</v>
@@ -1921,7 +1921,7 @@
         <v>p.hi zapzap</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>58</v>
@@ -1949,7 +1949,7 @@
         <v>p.hi patchi</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>11</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>61</v>
@@ -1977,7 +1977,7 @@
         <v>p.hi growela</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2005,15 +2005,15 @@
         <v>p.hi yopa</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>60</v>
@@ -2033,7 +2033,7 @@
         <v>p.hi mooshi</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>p.hi alidnak</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>61</v>
@@ -2089,7 +2089,7 @@
         <v>p.hi chickotik</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>p.hi gibut</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>59</v>
@@ -2145,7 +2145,7 @@
         <v>p.hi hooray</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>59</v>
@@ -2173,7 +2173,7 @@
         <v>p.hi magicilla</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>74</v>
@@ -2201,7 +2201,7 @@
         <v>p.hi balani</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>26</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>60</v>
@@ -2229,7 +2229,7 @@
         <v>p.hi chickama</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>59</v>
@@ -2257,7 +2257,7 @@
         <v>p.hi plok</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>61</v>
@@ -2305,9 +2305,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -2330,34 +2330,34 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
added aura to mythics
</commit_message>
<xml_diff>
--- a/Pokemon Supply Distribution.xlsx
+++ b/Pokemon Supply Distribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\00 - Projects\Dev\rumble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0690E5-CA23-404E-8508-F2270FD539EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD4146-E82E-4DA9-9888-0ABD64D0B514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C5DC818E-8AB9-4D02-86E9-8C9248B295A5}"/>
   </bookViews>
@@ -979,7 +979,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated readme with create commands
</commit_message>
<xml_diff>
--- a/Pokemon Supply Distribution.xlsx
+++ b/Pokemon Supply Distribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\00 - Projects\Dev\rumble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEB141E-4410-42E8-83E0-DE62757F8CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645EAAB9-AEC1-4FCE-AB0D-001D3F279E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C5DC818E-8AB9-4D02-86E9-8C9248B295A5}"/>
   </bookViews>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9966805-79DB-4CCA-A5D2-3255ED92FDD9}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>